<commit_message>
has been added ЕГЭ 15
</commit_message>
<xml_diff>
--- a/ЕГЭ Игнат Смотрицкий.xlsx
+++ b/ЕГЭ Игнат Смотрицкий.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C3F7B-FA0C-43B2-97D0-C09BB7C6D7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E674F253-AFD2-45DD-94C6-05983636E32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -786,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -798,11 +798,13 @@
     <col min="2" max="2" width="4.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="8"/>
+    <col min="5" max="5" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D1" s="14">
         <v>44848</v>
       </c>
@@ -810,8 +812,12 @@
         <v>44851</v>
       </c>
       <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="21">
+        <v>44857</v>
+      </c>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7">
         <v>1</v>
       </c>
@@ -819,8 +825,9 @@
         <v>0</v>
       </c>
       <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -829,7 +836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -838,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -851,8 +858,9 @@
       <c r="D5" s="17">
         <v>17320</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -863,8 +871,9 @@
         <v>4</v>
       </c>
       <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>4</v>
       </c>
@@ -872,8 +881,9 @@
         <v>5</v>
       </c>
       <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>5</v>
       </c>
@@ -882,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
@@ -891,7 +901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>5</v>
       </c>
@@ -899,8 +909,9 @@
         <v>8</v>
       </c>
       <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>7</v>
       </c>
@@ -909,7 +920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>8</v>
       </c>
@@ -918,7 +929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>9</v>
       </c>
@@ -929,8 +940,9 @@
         <v>61</v>
       </c>
       <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>7</v>
       </c>
@@ -938,8 +950,9 @@
         <v>11</v>
       </c>
       <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>10</v>
       </c>
@@ -947,7 +960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>11</v>
       </c>
@@ -955,7 +968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -963,7 +976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>8</v>
       </c>
@@ -971,8 +984,9 @@
         <v>15</v>
       </c>
       <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>13</v>
       </c>
@@ -980,7 +994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>14</v>
       </c>
@@ -988,7 +1002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>15</v>
       </c>
@@ -996,7 +1010,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>16</v>
       </c>
@@ -1009,8 +1023,9 @@
       <c r="D22" s="17">
         <v>27518</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>17</v>
       </c>
@@ -1021,8 +1036,9 @@
         <v>20</v>
       </c>
       <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
         <v>11</v>
       </c>
@@ -1030,8 +1046,9 @@
         <v>21</v>
       </c>
       <c r="D24" s="15"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>18</v>
       </c>
@@ -1040,7 +1057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>19</v>
       </c>
@@ -1049,7 +1066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>20</v>
       </c>
@@ -1060,8 +1077,9 @@
         <v>24</v>
       </c>
       <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
         <v>13</v>
       </c>
@@ -1069,8 +1087,9 @@
         <v>25</v>
       </c>
       <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>21</v>
       </c>
@@ -1079,7 +1098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>22</v>
       </c>
@@ -1088,7 +1107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>23</v>
       </c>
@@ -1097,7 +1116,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>24</v>
       </c>
@@ -1106,7 +1125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>25</v>
       </c>
@@ -1119,8 +1138,9 @@
       <c r="D33" s="18">
         <v>45248</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7">
         <v>15</v>
       </c>
@@ -1128,8 +1148,9 @@
         <v>31</v>
       </c>
       <c r="D34" s="15"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="15"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>26</v>
       </c>
@@ -1137,8 +1158,14 @@
       <c r="C35" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="4">
+        <v>38949</v>
+      </c>
+      <c r="H35" s="19">
+        <v>34516</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>27</v>
       </c>
@@ -1147,7 +1174,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>28</v>
       </c>
@@ -1156,7 +1183,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>29</v>
       </c>
@@ -1165,7 +1192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="7">
         <v>16</v>
       </c>
@@ -1173,8 +1200,9 @@
         <v>36</v>
       </c>
       <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="15"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>30</v>
       </c>
@@ -1183,7 +1211,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>31</v>
       </c>
@@ -1195,7 +1223,7 @@
         <v>38950</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>32</v>
       </c>
@@ -1204,7 +1232,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>33</v>
       </c>
@@ -1215,11 +1243,17 @@
         <v>40</v>
       </c>
       <c r="D43" s="15"/>
-      <c r="E43" s="19">
+      <c r="E43" s="4">
         <v>39762</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="18">
+        <v>37373</v>
+      </c>
+      <c r="G43" s="2">
+        <v>37372</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>34</v>
       </c>
@@ -1233,11 +1267,11 @@
       <c r="E44" s="4">
         <v>35992</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="18">
         <v>40734</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="7">
         <v>19</v>
       </c>
@@ -1245,8 +1279,9 @@
         <v>42</v>
       </c>
       <c r="D45" s="15"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="15"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>35</v>
       </c>
@@ -1255,7 +1290,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>36</v>
       </c>
@@ -1264,7 +1299,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
         <v>20</v>
       </c>
@@ -1272,8 +1307,9 @@
         <v>45</v>
       </c>
       <c r="D48" s="15"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F48" s="15"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>37</v>
       </c>
@@ -1282,7 +1318,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>38</v>
       </c>
@@ -1291,7 +1327,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="7">
         <v>21</v>
       </c>
@@ -1299,8 +1335,9 @@
         <v>46</v>
       </c>
       <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F51" s="15"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>39</v>
       </c>
@@ -1309,7 +1346,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>40</v>
       </c>
@@ -1318,7 +1355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="7">
         <v>22</v>
       </c>
@@ -1326,8 +1363,9 @@
         <v>62</v>
       </c>
       <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="15"/>
+    </row>
+    <row r="55" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7">
         <v>23</v>
       </c>
@@ -1335,8 +1373,9 @@
         <v>47</v>
       </c>
       <c r="D55" s="15"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F55" s="15"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>45</v>
       </c>
@@ -1345,7 +1384,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>46</v>
       </c>
@@ -1354,7 +1393,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>47</v>
       </c>
@@ -1363,7 +1402,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>48</v>
       </c>
@@ -1372,7 +1411,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>49</v>
       </c>
@@ -1383,8 +1422,9 @@
         <v>52</v>
       </c>
       <c r="D60" s="15"/>
-    </row>
-    <row r="61" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="15"/>
+    </row>
+    <row r="61" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>50</v>
       </c>
@@ -1395,8 +1435,9 @@
         <v>53</v>
       </c>
       <c r="D61" s="15"/>
-    </row>
-    <row r="62" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="15"/>
+    </row>
+    <row r="62" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>51</v>
       </c>
@@ -1407,8 +1448,9 @@
         <v>53</v>
       </c>
       <c r="D62" s="15"/>
-    </row>
-    <row r="63" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F62" s="15"/>
+    </row>
+    <row r="63" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>52</v>
       </c>
@@ -1419,8 +1461,9 @@
         <v>54</v>
       </c>
       <c r="D63" s="15"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F63" s="15"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="9"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
@@ -1436,8 +1479,9 @@
       <c r="B68" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" display="https://inf-ege.sdamgia.ru/problem?id=17320" xr:uid="{6E199988-EFAE-4001-8D50-712F42EA03C9}"/>
@@ -1447,9 +1491,13 @@
     <hyperlink ref="E44" r:id="rId5" display="https://inf-ege.sdamgia.ru/problem?id=35992" xr:uid="{F0FA48CC-6AE3-4EE5-8873-E7DE45BEE9F6}"/>
     <hyperlink ref="F44" r:id="rId6" display="https://inf-ege.sdamgia.ru/problem?id=40734" xr:uid="{08D51E11-A14B-4204-A605-16D35C95F962}"/>
     <hyperlink ref="E43" r:id="rId7" display="https://inf-ege.sdamgia.ru/problem?id=39762" xr:uid="{02E1BDCD-1E3E-4EAD-9ED7-1C423757F4A2}"/>
+    <hyperlink ref="G43" r:id="rId8" display="https://inf-ege.sdamgia.ru/problem?id=37372" xr:uid="{B606E77D-BEEE-4177-B2BC-789E1B5F0C13}"/>
+    <hyperlink ref="F43" r:id="rId9" display="https://inf-ege.sdamgia.ru/problem?id=37373" xr:uid="{511EDE11-A2CF-485D-A3B8-90E7197FEC35}"/>
+    <hyperlink ref="G35" r:id="rId10" display="https://inf-ege.sdamgia.ru/problem?id=38949" xr:uid="{F4034074-E614-45C3-BED2-EE660733B254}"/>
+    <hyperlink ref="H35" r:id="rId11" display="https://inf-ege.sdamgia.ru/problem?id=34516" xr:uid="{B37012A6-9CBB-4F60-B6E6-70EEA6E85900}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
has been added ЕГЭ 8
</commit_message>
<xml_diff>
--- a/ЕГЭ Игнат Смотрицкий.xlsx
+++ b/ЕГЭ Игнат Смотрицкий.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E674F253-AFD2-45DD-94C6-05983636E32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AE10DA-CC55-4A8E-8E3D-81528568D618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -968,7 +968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -976,7 +976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>8</v>
       </c>
@@ -986,7 +986,7 @@
       <c r="D18" s="15"/>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>13</v>
       </c>
@@ -994,23 +994,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>14</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="19">
+        <v>36021</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>15</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="2">
+        <v>5087</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>16</v>
       </c>
@@ -1025,7 +1031,7 @@
       </c>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>17</v>
       </c>
@@ -1038,7 +1044,7 @@
       <c r="D23" s="15"/>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
         <v>11</v>
       </c>
@@ -1048,7 +1054,7 @@
       <c r="D24" s="15"/>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>18</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>19</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>20</v>
       </c>
@@ -1079,7 +1085,7 @@
       <c r="D27" s="15"/>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
         <v>13</v>
       </c>
@@ -1089,7 +1095,7 @@
       <c r="D28" s="15"/>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>21</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>22</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>23</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>24</v>
       </c>
@@ -1124,6 +1130,9 @@
       <c r="C32" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="G32" s="2">
+        <v>33483</v>
+      </c>
     </row>
     <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
@@ -1139,6 +1148,9 @@
         <v>45248</v>
       </c>
       <c r="F33" s="15"/>
+      <c r="G33" s="2">
+        <v>38948</v>
+      </c>
     </row>
     <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="7">
@@ -1161,7 +1173,7 @@
       <c r="G35" s="4">
         <v>38949</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H35" s="1">
         <v>34516</v>
       </c>
     </row>
@@ -1181,6 +1193,9 @@
       <c r="B37" s="9"/>
       <c r="C37" s="12" t="s">
         <v>34</v>
+      </c>
+      <c r="G37" s="2">
+        <v>16821</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1495,9 +1510,14 @@
     <hyperlink ref="F43" r:id="rId9" display="https://inf-ege.sdamgia.ru/problem?id=37373" xr:uid="{511EDE11-A2CF-485D-A3B8-90E7197FEC35}"/>
     <hyperlink ref="G35" r:id="rId10" display="https://inf-ege.sdamgia.ru/problem?id=38949" xr:uid="{F4034074-E614-45C3-BED2-EE660733B254}"/>
     <hyperlink ref="H35" r:id="rId11" display="https://inf-ege.sdamgia.ru/problem?id=34516" xr:uid="{B37012A6-9CBB-4F60-B6E6-70EEA6E85900}"/>
+    <hyperlink ref="G37" r:id="rId12" display="https://inf-ege.sdamgia.ru/problem?id=16821" xr:uid="{3032177C-B964-47A6-BE8A-990902AE2EF1}"/>
+    <hyperlink ref="G33" r:id="rId13" display="https://inf-ege.sdamgia.ru/problem?id=38948" xr:uid="{D8663CF8-2A89-4AED-9DBE-C3CED4AB1BF9}"/>
+    <hyperlink ref="G32" r:id="rId14" display="https://inf-ege.sdamgia.ru/problem?id=33483" xr:uid="{3A489FB2-C069-4DF9-B32A-62CE1C38B726}"/>
+    <hyperlink ref="G21" r:id="rId15" display="https://inf-ege.sdamgia.ru/problem?id=5087" xr:uid="{06A3A6BD-08B9-4334-AA4C-D18D7F8C0C42}"/>
+    <hyperlink ref="G20" r:id="rId16" display="https://inf-ege.sdamgia.ru/problem?id=36021" xr:uid="{75535224-1F34-4342-B850-06073954A690}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>